<commit_message>
modified in the local
</commit_message>
<xml_diff>
--- a/Collections/Test_Data/TestData.xlsx
+++ b/Collections/Test_Data/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>added from local git</t>
   </si>
 </sst>
 </file>
@@ -378,15 +381,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -397,7 +400,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -406,6 +409,9 @@
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified exce in local
</commit_message>
<xml_diff>
--- a/Collections/Test_Data/TestData.xlsx
+++ b/Collections/Test_Data/TestData.xlsx
@@ -39,7 +39,7 @@
     <t>added from local git</t>
   </si>
   <si>
-    <t>Modified on master</t>
+    <t>Modified on local</t>
   </si>
 </sst>
 </file>
@@ -387,7 +387,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>